<commit_message>
Update layout espace admin
</commit_message>
<xml_diff>
--- a/Etudiants.xlsx
+++ b/Etudiants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\4eme\.Net Projects\Projet.NetCore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E13E94C-75A6-48CD-9261-81059A2FC538}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECF8B92-2332-43B1-BFB9-A919D4AE21AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7CF774BF-FDFD-476E-A34D-F750F3FBC6FB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12516" xr2:uid="{7CF774BF-FDFD-476E-A34D-F750F3FBC6FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -302,6 +302,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -314,14 +382,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="DEDEDE"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="181B28"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -612,17 +680,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{664942CC-5715-447F-88C0-96923341BDC3}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" zoomScale="128" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>27</v>
       </c>
@@ -633,20 +701,20 @@
         <v>29</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1230</v>
       </c>
@@ -657,20 +725,20 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>1</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1231</v>
       </c>
@@ -681,20 +749,20 @@
         <v>4</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4">
+      <c r="H3" s="4">
         <v>1</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1232</v>
       </c>
@@ -704,21 +772,21 @@
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>1</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>1233</v>
       </c>
@@ -729,20 +797,20 @@
         <v>10</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4">
+      <c r="H5" s="4">
         <v>1</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1236</v>
       </c>
@@ -752,21 +820,21 @@
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>1</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>1237</v>
       </c>
@@ -777,20 +845,20 @@
         <v>16</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4">
+      <c r="H7" s="4">
         <v>1</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1238</v>
       </c>
@@ -800,21 +868,21 @@
       <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>1</v>
       </c>
-      <c r="H8" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>1239</v>
       </c>
@@ -825,20 +893,20 @@
         <v>22</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4">
+      <c r="H9" s="4">
         <v>1</v>
       </c>
-      <c r="H9" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>1240</v>
       </c>
@@ -848,21 +916,21 @@
       <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>2</v>
       </c>
-      <c r="H10" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>1241</v>
       </c>
@@ -873,17 +941,17 @@
         <v>33</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4">
+      <c r="H11" s="4">
         <v>2</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>